<commit_message>
export: Update conditional formatting
</commit_message>
<xml_diff>
--- a/export/v1.0.6a/techtree.xlsx
+++ b/export/v1.0.6a/techtree.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2025\games\microtopia\export-manual\v1.0.6a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data\2025\pwsh\MicrotopiaData\export\v1.0.6a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A193A67F-2CF7-4494-80E9-298571F57A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A30BAC-9204-4C99-85E3-506D5F23D774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15394" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="2685" windowWidth="27240" windowHeight="16950" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TechTree" sheetId="4" r:id="rId1"/>
@@ -1608,7 +1608,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1852,25 +1863,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4AB7FF-4C2C-4E6B-B1CD-14A37677CFE6}">
   <dimension ref="A1:O321"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J297" sqref="J297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.921875" customWidth="1"/>
-    <col min="5" max="5" width="12.69140625" customWidth="1"/>
-    <col min="6" max="6" width="9.4609375" customWidth="1"/>
+    <col min="1" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="22.3828125" customWidth="1"/>
-    <col min="12" max="12" width="14.3046875" customWidth="1"/>
-    <col min="13" max="13" width="10.69140625" customWidth="1"/>
-    <col min="14" max="14" width="15.53515625" customWidth="1"/>
-    <col min="15" max="15" width="13.4609375" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1917,22 +1931,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1949,7 +1963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1969,7 +1983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1986,7 +2000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2003,7 +2017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2020,7 +2034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2037,7 +2051,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2057,7 +2071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2074,7 +2088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2091,7 +2105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2108,7 +2122,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2139,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2142,7 +2156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2162,7 +2176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2182,7 +2196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -2202,7 +2216,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -2219,7 +2233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -2236,7 +2250,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2253,7 +2267,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -2270,7 +2284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2287,7 +2301,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -2304,7 +2318,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2321,7 +2335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -2338,7 +2352,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>95</v>
       </c>
@@ -2355,7 +2369,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2372,12 +2386,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -2394,7 +2408,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -2411,7 +2425,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -2428,7 +2442,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2445,7 +2459,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -2462,7 +2476,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>116</v>
       </c>
@@ -2485,7 +2499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2502,7 +2516,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -2522,7 +2536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -2539,12 +2553,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2561,7 +2575,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2578,7 +2592,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>131</v>
       </c>
@@ -2595,7 +2609,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>134</v>
       </c>
@@ -2612,7 +2626,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2629,7 +2643,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -2646,7 +2660,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>139</v>
       </c>
@@ -2663,7 +2677,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>142</v>
       </c>
@@ -2683,7 +2697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -2700,7 +2714,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -2717,7 +2731,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2734,7 +2748,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -2751,12 +2765,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>151</v>
       </c>
@@ -2773,7 +2787,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>155</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>158</v>
       </c>
@@ -2813,7 +2827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>152</v>
       </c>
@@ -2833,7 +2847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>161</v>
       </c>
@@ -2850,7 +2864,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>164</v>
       </c>
@@ -2867,7 +2881,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>166</v>
       </c>
@@ -2884,7 +2898,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>168</v>
       </c>
@@ -2901,7 +2915,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>171</v>
       </c>
@@ -2918,7 +2932,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -2935,7 +2949,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>173</v>
       </c>
@@ -2955,7 +2969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2972,7 +2986,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2989,12 +3003,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>181</v>
       </c>
@@ -3017,7 +3031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>184</v>
       </c>
@@ -3037,7 +3051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>185</v>
       </c>
@@ -3057,12 +3071,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -3073,7 +3087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>189</v>
       </c>
@@ -3087,7 +3101,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -3104,7 +3118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -3121,7 +3135,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>58</v>
       </c>
@@ -3138,7 +3152,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -3155,7 +3169,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>140</v>
       </c>
@@ -3172,7 +3186,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -3189,7 +3203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>110</v>
       </c>
@@ -3206,7 +3220,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>129</v>
       </c>
@@ -3223,7 +3237,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>66</v>
       </c>
@@ -3240,7 +3254,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>132</v>
       </c>
@@ -3257,7 +3271,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>178</v>
       </c>
@@ -3274,7 +3288,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -3294,7 +3308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>49</v>
       </c>
@@ -3311,7 +3325,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>145</v>
       </c>
@@ -3328,7 +3342,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -3345,7 +3359,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>29</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -3379,7 +3393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>89</v>
       </c>
@@ -3396,7 +3410,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -3413,7 +3427,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -3430,12 +3444,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>192</v>
       </c>
@@ -3452,7 +3466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>194</v>
       </c>
@@ -3466,7 +3480,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>195</v>
       </c>
@@ -3480,7 +3494,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>196</v>
       </c>
@@ -3494,7 +3508,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>197</v>
       </c>
@@ -3508,7 +3522,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>198</v>
       </c>
@@ -3522,7 +3536,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>199</v>
       </c>
@@ -3536,7 +3550,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>200</v>
       </c>
@@ -3550,7 +3564,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>201</v>
       </c>
@@ -3564,17 +3578,17 @@
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>203</v>
       </c>
@@ -3591,7 +3605,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>207</v>
       </c>
@@ -3608,7 +3622,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>211</v>
       </c>
@@ -3625,7 +3639,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>215</v>
       </c>
@@ -3642,7 +3656,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>218</v>
       </c>
@@ -3659,7 +3673,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>221</v>
       </c>
@@ -3676,7 +3690,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>222</v>
       </c>
@@ -3693,7 +3707,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>226</v>
       </c>
@@ -3710,7 +3724,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>228</v>
       </c>
@@ -3727,7 +3741,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>231</v>
       </c>
@@ -3744,7 +3758,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>234</v>
       </c>
@@ -3761,7 +3775,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -3778,7 +3792,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>241</v>
       </c>
@@ -3795,7 +3809,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>245</v>
       </c>
@@ -3812,7 +3826,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>249</v>
       </c>
@@ -3829,7 +3843,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>253</v>
       </c>
@@ -3846,7 +3860,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>256</v>
       </c>
@@ -3863,7 +3877,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>510</v>
       </c>
@@ -3880,12 +3894,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>242</v>
       </c>
@@ -3902,7 +3916,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>265</v>
       </c>
@@ -3919,7 +3933,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>267</v>
       </c>
@@ -3936,7 +3950,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>271</v>
       </c>
@@ -3953,7 +3967,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>262</v>
       </c>
@@ -3970,7 +3984,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>275</v>
       </c>
@@ -3987,7 +4001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>277</v>
       </c>
@@ -4004,7 +4018,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>280</v>
       </c>
@@ -4021,7 +4035,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>283</v>
       </c>
@@ -4038,7 +4052,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>286</v>
       </c>
@@ -4055,12 +4069,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>290</v>
       </c>
@@ -4077,12 +4091,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>292</v>
       </c>
@@ -4099,7 +4113,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>212</v>
       </c>
@@ -4116,7 +4130,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>208</v>
       </c>
@@ -4133,7 +4147,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>298</v>
       </c>
@@ -4150,7 +4164,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>300</v>
       </c>
@@ -4167,7 +4181,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>303</v>
       </c>
@@ -4184,7 +4198,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>281</v>
       </c>
@@ -4201,7 +4215,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>284</v>
       </c>
@@ -4218,7 +4232,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>287</v>
       </c>
@@ -4235,7 +4249,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>312</v>
       </c>
@@ -4252,7 +4266,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>314</v>
       </c>
@@ -4269,7 +4283,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>316</v>
       </c>
@@ -4286,7 +4300,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>318</v>
       </c>
@@ -4309,7 +4323,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>229</v>
       </c>
@@ -4326,7 +4340,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>319</v>
       </c>
@@ -4343,7 +4357,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>238</v>
       </c>
@@ -4360,7 +4374,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>304</v>
       </c>
@@ -4377,12 +4391,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>268</v>
       </c>
@@ -4399,7 +4413,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>306</v>
       </c>
@@ -4416,7 +4430,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>257</v>
       </c>
@@ -4433,7 +4447,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>331</v>
       </c>
@@ -4450,7 +4464,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>308</v>
       </c>
@@ -4467,7 +4481,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>310</v>
       </c>
@@ -4484,7 +4498,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>204</v>
       </c>
@@ -4501,7 +4515,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>294</v>
       </c>
@@ -4518,7 +4532,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>219</v>
       </c>
@@ -4535,7 +4549,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>246</v>
       </c>
@@ -4552,7 +4566,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>250</v>
       </c>
@@ -4569,7 +4583,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>235</v>
       </c>
@@ -4586,7 +4600,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>328</v>
       </c>
@@ -4603,7 +4617,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>330</v>
       </c>
@@ -4620,7 +4634,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>232</v>
       </c>
@@ -4637,7 +4651,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>273</v>
       </c>
@@ -4654,12 +4668,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>333</v>
       </c>
@@ -4673,7 +4687,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>334</v>
       </c>
@@ -4687,7 +4701,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>335</v>
       </c>
@@ -4701,7 +4715,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>336</v>
       </c>
@@ -4715,7 +4729,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>337</v>
       </c>
@@ -4729,7 +4743,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>338</v>
       </c>
@@ -4743,7 +4757,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>339</v>
       </c>
@@ -4757,7 +4771,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>340</v>
       </c>
@@ -4771,7 +4785,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>341</v>
       </c>
@@ -4785,7 +4799,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>342</v>
       </c>
@@ -4799,7 +4813,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>343</v>
       </c>
@@ -4813,17 +4827,17 @@
         <v>343</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>511</v>
       </c>
@@ -4840,7 +4854,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>348</v>
       </c>
@@ -4857,7 +4871,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>351</v>
       </c>
@@ -4874,7 +4888,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>355</v>
       </c>
@@ -4891,7 +4905,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -4908,7 +4922,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>512</v>
       </c>
@@ -4922,12 +4936,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>352</v>
       </c>
@@ -4944,7 +4958,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>364</v>
       </c>
@@ -4961,7 +4975,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>368</v>
       </c>
@@ -4978,7 +4992,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>370</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>374</v>
       </c>
@@ -5012,7 +5026,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>376</v>
       </c>
@@ -5029,12 +5043,12 @@
         <v>379</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>380</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>383</v>
       </c>
@@ -5068,7 +5082,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>345</v>
       </c>
@@ -5085,7 +5099,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>377</v>
       </c>
@@ -5102,12 +5116,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>365</v>
       </c>
@@ -5124,7 +5138,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>349</v>
       </c>
@@ -5141,7 +5155,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>361</v>
       </c>
@@ -5158,7 +5172,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>381</v>
       </c>
@@ -5175,7 +5189,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>371</v>
       </c>
@@ -5192,12 +5206,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>389</v>
       </c>
@@ -5211,7 +5225,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>390</v>
       </c>
@@ -5225,7 +5239,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>391</v>
       </c>
@@ -5239,7 +5253,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>392</v>
       </c>
@@ -5253,7 +5267,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>393</v>
       </c>
@@ -5267,17 +5281,17 @@
         <v>393</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>395</v>
       </c>
@@ -5291,7 +5305,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>397</v>
       </c>
@@ -5305,7 +5319,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>399</v>
       </c>
@@ -5316,7 +5330,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>400</v>
       </c>
@@ -5327,7 +5341,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>402</v>
       </c>
@@ -5338,7 +5352,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>404</v>
       </c>
@@ -5349,7 +5363,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>405</v>
       </c>
@@ -5360,7 +5374,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>407</v>
       </c>
@@ -5371,22 +5385,22 @@
         <v>408</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>409</v>
       </c>
@@ -5400,7 +5414,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>410</v>
       </c>
@@ -5414,7 +5428,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>411</v>
       </c>
@@ -5428,12 +5442,12 @@
         <v>411</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>413</v>
       </c>
@@ -5441,17 +5455,17 @@
         <v>414</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>416</v>
       </c>
@@ -5465,7 +5479,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>418</v>
       </c>
@@ -5479,7 +5493,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>420</v>
       </c>
@@ -5493,7 +5507,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>422</v>
       </c>
@@ -5504,7 +5518,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>423</v>
       </c>
@@ -5515,7 +5529,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>425</v>
       </c>
@@ -5526,7 +5540,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>427</v>
       </c>
@@ -5540,7 +5554,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>430</v>
       </c>
@@ -5551,7 +5565,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>513</v>
       </c>
@@ -5562,17 +5576,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>432</v>
       </c>
@@ -5583,7 +5597,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>433</v>
       </c>
@@ -5594,7 +5608,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>434</v>
       </c>
@@ -5605,7 +5619,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>435</v>
       </c>
@@ -5616,12 +5630,12 @@
         <v>431</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>436</v>
       </c>
@@ -5635,7 +5649,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>437</v>
       </c>
@@ -5649,12 +5663,12 @@
         <v>437</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>438</v>
       </c>
@@ -5662,7 +5676,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>439</v>
       </c>
@@ -5670,17 +5684,17 @@
         <v>426</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>441</v>
       </c>
@@ -5694,7 +5708,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>444</v>
       </c>
@@ -5705,7 +5719,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>445</v>
       </c>
@@ -5719,7 +5733,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>446</v>
       </c>
@@ -5733,12 +5747,12 @@
         <v>447</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>448</v>
       </c>
@@ -5752,7 +5766,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>450</v>
       </c>
@@ -5766,7 +5780,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>452</v>
       </c>
@@ -5777,7 +5791,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>453</v>
       </c>
@@ -5797,7 +5811,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>458</v>
       </c>
@@ -5817,7 +5831,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>462</v>
       </c>
@@ -5831,17 +5845,17 @@
         <v>463</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>464</v>
       </c>
@@ -5855,7 +5869,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>466</v>
       </c>
@@ -5866,12 +5880,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>468</v>
       </c>
@@ -5882,7 +5896,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>469</v>
       </c>
@@ -5893,7 +5907,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>470</v>
       </c>
@@ -5904,7 +5918,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>471</v>
       </c>
@@ -5915,7 +5929,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>472</v>
       </c>
@@ -5926,7 +5940,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>473</v>
       </c>
@@ -5938,6 +5952,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:O321">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5949,18 +5968,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF6EA8C-5336-4A81-A2BD-D675BD018144}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.15234375" customWidth="1"/>
-    <col min="6" max="6" width="11.61328125" customWidth="1"/>
-    <col min="7" max="7" width="21.23046875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5983,7 +6006,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>479</v>
       </c>
@@ -6003,7 +6026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>482</v>
       </c>
@@ -6020,7 +6043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>484</v>
       </c>
@@ -6037,7 +6060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>486</v>
       </c>
@@ -6054,7 +6077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>489</v>
       </c>
@@ -6071,7 +6094,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>491</v>
       </c>
@@ -6088,7 +6111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>493</v>
       </c>
@@ -6105,7 +6128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>496</v>
       </c>
@@ -6122,7 +6145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>498</v>
       </c>
@@ -6140,10 +6163,66 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CC0D4A07-E8AD-44D9-A407-088BB325BB0A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C8549FA9-CA0D-448A-A9C7-53DC5B77AEFD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CC0D4A07-E8AD-44D9-A407-088BB325BB0A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G2:G10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C8549FA9-CA0D-448A-A9C7-53DC5B77AEFD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E2:E10</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6151,17 +6230,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473F5FDB-1BD0-43AA-83AD-1260B626325F}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="96.07421875" customWidth="1"/>
+    <col min="2" max="2" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>500</v>
       </c>
@@ -6169,7 +6246,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6177,7 +6254,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6185,7 +6262,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6193,7 +6270,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6201,7 +6278,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6209,7 +6286,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6217,7 +6294,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6225,7 +6302,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6233,7 +6310,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -6241,7 +6318,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -6249,7 +6326,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -6257,7 +6334,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -6265,7 +6342,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -6273,7 +6350,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -6281,7 +6358,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -6289,7 +6366,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -6297,7 +6374,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -6305,7 +6382,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -6313,7 +6390,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -6321,7 +6398,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -6329,7 +6406,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -6337,7 +6414,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -6345,7 +6422,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -6353,7 +6430,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -6361,7 +6438,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -6369,7 +6446,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -6377,7 +6454,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -6385,7 +6462,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -6393,7 +6470,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -6401,7 +6478,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -6409,7 +6486,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -6417,7 +6494,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -6425,7 +6502,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -6433,7 +6510,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -6441,7 +6518,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6449,7 +6526,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6457,7 +6534,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6465,7 +6542,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6473,7 +6550,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6481,7 +6558,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6489,7 +6566,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6497,7 +6574,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6505,7 +6582,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6513,7 +6590,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6521,7 +6598,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6529,7 +6606,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6537,7 +6614,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6545,7 +6622,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6553,7 +6630,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6561,7 +6638,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>

</xml_diff>